<commit_message>
app controller and junit
</commit_message>
<xml_diff>
--- a/uml/systemtests/CIT360 - System Level Test Cleanup.xlsx
+++ b/uml/systemtests/CIT360 - System Level Test Cleanup.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d0dc1a3df7cb25e/Documents/BYUI/CIT360/cit360/uml/systemtests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mythr\OneDrive\Documents\BYUI\CIT360\cit360\uml\systemtests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{84086395-EB13-4509-BBC5-57BEEF8BC6E2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{BB489A53-F050-4243-8382-E4EBDF9CE8D7}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{84086395-EB13-4509-BBC5-57BEEF8BC6E2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{CF56F181-AB81-444F-BF95-2B650B1A3118}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8423" windowHeight="3893" xr2:uid="{A3D11415-B1AF-4E17-A9B6-68F2C84933C2}"/>
   </bookViews>
@@ -268,31 +268,31 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,236 +613,236 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.46484375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.19921875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="12"/>
+      <c r="C4" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="8" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="2"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="10" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="2"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="13">
+      <c r="A8" s="8">
         <v>1</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="13">
+      <c r="A9" s="8">
         <v>2</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" s="13">
+      <c r="A10" s="8">
         <v>3</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" s="13">
+      <c r="A11" s="8">
         <v>5</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" s="13">
+      <c r="A12" s="8">
         <v>6</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="13">
+      <c r="A13" s="8">
         <v>7</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" s="13">
+      <c r="A14" s="8">
         <v>8</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="13">
+      <c r="A15" s="8">
         <v>9</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>